<commit_message>
working on yutaka, updated rankings
</commit_message>
<xml_diff>
--- a/resources/_rankings.xlsx
+++ b/resources/_rankings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Other\Coding\oii2021\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE3EFA98-6995-40F7-814D-0CB4E055FBC1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FBBA5B3-AB21-4FA0-A4E2-8DCCE285A0CA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1440" yWindow="1635" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -352,10 +352,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,6 +441,28 @@
         <v>-1723</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>44312</v>
+      </c>
+      <c r="B8">
+        <v>84</v>
+      </c>
+      <c r="C8">
+        <v>-1723</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>44313</v>
+      </c>
+      <c r="B9">
+        <v>96</v>
+      </c>
+      <c r="C9">
+        <v>-1553</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>